<commit_message>
Update modal split indicator so that Green Party removed as a source
</commit_message>
<xml_diff>
--- a/datastatic/datasets/online/SDG11_Modalsplit_passenger_transport_Trains_EUROSTAT_2014.xlsx
+++ b/datastatic/datasets/online/SDG11_Modalsplit_passenger_transport_Trains_EUROSTAT_2014.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="88">
   <si>
     <t>original_title</t>
   </si>
@@ -154,6 +154,9 @@
     <t>source$note</t>
   </si>
   <si>
+    <t>This indicator is also proposed by the German Green party</t>
+  </si>
+  <si>
     <t>source$publisher</t>
   </si>
   <si>
@@ -169,13 +172,10 @@
     <t>source$value</t>
   </si>
   <si>
-    <t>OKF, Bundestagsfraktion der Grünen</t>
+    <t>OKF</t>
   </si>
   <si>
     <t>source$maintainer</t>
-  </si>
-  <si>
-    <t>OKF</t>
   </si>
   <si>
     <t>source$license</t>
@@ -628,38 +628,40 @@
       <c r="A30" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="2"/>
+      <c r="B30" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="35">

</xml_diff>